<commit_message>
Add the generation scripts and the excel table for pumps
</commit_message>
<xml_diff>
--- a/pumps_table.xlsx
+++ b/pumps_table.xlsx
@@ -397,11 +397,11 @@
   </sheetPr>
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S10" activeCellId="0" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.86"/>
@@ -627,12 +627,12 @@
         <v>38</v>
       </c>
       <c r="R3" s="0" t="n">
-        <f aca="false">(M3-L3)/(P3-O3)</f>
-        <v>7.26190476190476</v>
+        <f aca="false">(P3-O3)/(M3-L3)</f>
+        <v>0.137704918032787</v>
       </c>
       <c r="S3" s="0" t="n">
-        <f aca="false">M3-(R3*P3)</f>
-        <v>1.54761904761904</v>
+        <f aca="false">P3-(R3*M3)</f>
+        <v>-0.213114754098351</v>
       </c>
       <c r="T3" s="0" t="s">
         <v>39</v>
@@ -714,12 +714,12 @@
         <v>38</v>
       </c>
       <c r="R4" s="0" t="n">
-        <f aca="false">(M4-L4)/(P4-O4)</f>
-        <v>4.76190476190476</v>
+        <f aca="false">(P4-O4)/(M4-L4)</f>
+        <v>0.21</v>
       </c>
       <c r="S4" s="0" t="n">
-        <f aca="false">M4-(R4*P4)</f>
-        <v>9.04761904761906</v>
+        <f aca="false">P4-(R4*M4)</f>
+        <v>-1.89999999999998</v>
       </c>
       <c r="T4" s="0" t="s">
         <v>39</v>
@@ -801,12 +801,12 @@
         <v>38</v>
       </c>
       <c r="R5" s="0" t="n">
-        <f aca="false">(M5-L5)/(P5-O5)</f>
-        <v>3.33333333333333</v>
+        <f aca="false">(P5-O5)/(M5-L5)</f>
+        <v>0.299999999999999</v>
       </c>
       <c r="S5" s="0" t="n">
-        <f aca="false">M5-(R5*P5)</f>
-        <v>13.3333333333333</v>
+        <f aca="false">P5-(R5*M5)</f>
+        <v>-3.99999999999997</v>
       </c>
       <c r="T5" s="0" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Pump Scripts | Update the scripts and the pumps_table.xlsx to the new convention for actuators
</commit_message>
<xml_diff>
--- a/pumps_table.xlsx
+++ b/pumps_table.xlsx
@@ -55,28 +55,28 @@
     <t xml:space="preserve">Netzanschluss</t>
   </si>
   <si>
-    <t xml:space="preserve">Ausgabebereich von</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabebereich bis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabebereich Einheit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eingabebereich von</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eingabebereich bis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eingabebereich Einheit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kennlinie Steigung _ Sensitivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kennlinie Offset _ Bias</t>
+    <t xml:space="preserve">Actuator Input Range from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuator Input Range to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuator Input Range unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuator Actuation Range from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuator Actuation Range to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuator Actuation Range unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuator Kennlinie _ Sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuator Kennlinie _ Bias</t>
   </si>
   <si>
     <t xml:space="preserve">Hersteller</t>
@@ -133,10 +133,10 @@
     <t xml:space="preserve">1~230 V, 50/60 Hz</t>
   </si>
   <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
     <t xml:space="preserve">1/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V</t>
   </si>
   <si>
     <t xml:space="preserve">WILO</t>
@@ -397,11 +397,11 @@
   </sheetPr>
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S10" activeCellId="0" sqref="S10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.86"/>
@@ -473,22 +473,22 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="3" t="s">
@@ -552,12 +552,12 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
       <c r="T2" s="1"/>
@@ -607,32 +607,32 @@
         <v>36</v>
       </c>
       <c r="L3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="0" t="n">
         <f aca="false">1400/60</f>
         <v>23.3333333333333</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="P3" s="0" t="n">
         <f aca="false">4450/60</f>
         <v>74.1666666666667</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>10</v>
-      </c>
       <c r="Q3" s="0" t="s">
         <v>38</v>
       </c>
       <c r="R3" s="0" t="n">
-        <f aca="false">(P3-O3)/(M3-L3)</f>
+        <f aca="false">(M3-L3)/(P3-O3)</f>
         <v>0.137704918032787</v>
       </c>
       <c r="S3" s="0" t="n">
-        <f aca="false">P3-(R3*M3)</f>
-        <v>-0.213114754098351</v>
+        <f aca="false">M3-(R3*P3)</f>
+        <v>-0.21311475409836</v>
       </c>
       <c r="T3" s="0" t="s">
         <v>39</v>
@@ -694,32 +694,32 @@
         <v>36</v>
       </c>
       <c r="L4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="0" t="n">
         <f aca="false">1400/60</f>
         <v>23.3333333333333</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="P4" s="0" t="n">
         <f aca="false">3400/60</f>
         <v>56.6666666666667</v>
       </c>
-      <c r="N4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P4" s="0" t="n">
-        <v>10</v>
-      </c>
       <c r="Q4" s="0" t="s">
         <v>38</v>
       </c>
       <c r="R4" s="0" t="n">
-        <f aca="false">(P4-O4)/(M4-L4)</f>
+        <f aca="false">(M4-L4)/(P4-O4)</f>
         <v>0.21</v>
       </c>
       <c r="S4" s="0" t="n">
-        <f aca="false">P4-(R4*M4)</f>
-        <v>-1.89999999999998</v>
+        <f aca="false">M4-(R4*P4)</f>
+        <v>-1.9</v>
       </c>
       <c r="T4" s="0" t="s">
         <v>39</v>
@@ -781,32 +781,32 @@
         <v>36</v>
       </c>
       <c r="L5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="0" t="n">
         <f aca="false">1400/60</f>
         <v>23.3333333333333</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="P5" s="0" t="n">
         <f aca="false">2800/60</f>
         <v>46.6666666666667</v>
       </c>
-      <c r="N5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="O5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P5" s="0" t="n">
-        <v>10</v>
-      </c>
       <c r="Q5" s="0" t="s">
         <v>38</v>
       </c>
       <c r="R5" s="0" t="n">
-        <f aca="false">(P5-O5)/(M5-L5)</f>
-        <v>0.299999999999999</v>
+        <f aca="false">(M5-L5)/(P5-O5)</f>
+        <v>0.3</v>
       </c>
       <c r="S5" s="0" t="n">
-        <f aca="false">P5-(R5*M5)</f>
-        <v>-3.99999999999997</v>
+        <f aca="false">M5-(R5*P5)</f>
+        <v>-4</v>
       </c>
       <c r="T5" s="0" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Add the updated pumps_table.xlsx
</commit_message>
<xml_diff>
--- a/pumps_table.xlsx
+++ b/pumps_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t xml:space="preserve">uuid</t>
   </si>
@@ -61,6 +61,12 @@
     <t xml:space="preserve">Actuator Input Range to</t>
   </si>
   <si>
+    <t xml:space="preserve">Actuator Input Range _ sluggishness zone from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuator Input Range _ sluggishness zone to</t>
+  </si>
+  <si>
     <t xml:space="preserve">Actuator Input Range unit</t>
   </si>
   <si>
@@ -160,7 +166,7 @@
     <t xml:space="preserve">Frequenzumrichter IF-Modul-Strator</t>
   </si>
   <si>
-    <t xml:space="preserve">Montageort: Pumpe 1</t>
+    <t xml:space="preserve">Montageort: Pumpe 1; The actuator actuation sensitivity and bias is only calculated for a actuator actuation input range of 3 V - 10 V, since the 3 V is the minimal amount of voltage needed to get the pump to work</t>
   </si>
   <si>
     <t xml:space="preserve">0193081d-0a01-7b16-90d8-c1dd16e31672</t>
@@ -172,7 +178,7 @@
     <t xml:space="preserve">..\3_Konzipieren und Konstruieren\Datenblaetter\info_240917_Datenblatt_Pumpe_Wilo_Stratos_25_1-6.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">Montageort: Pumpe 2</t>
+    <t xml:space="preserve">Montageort: Pumpe 2; The actuator actuation sensitivity and bias is only calculated for a actuator actuation input range of 3 V - 10 V, since the 3 V is the minimal amount of voltage needed to get the pump to work</t>
   </si>
   <si>
     <t xml:space="preserve">0193081d-0a02-74ba-9f80-01f28979b926</t>
@@ -184,7 +190,7 @@
     <t xml:space="preserve">..\3_Konzipieren und Konstruieren\Datenblaetter\info_241024_Datenblatt_Pumpe_Wilo_Stratos_25_1-4.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">Nicht verbaut</t>
+    <t xml:space="preserve">Nicht verbaut;  The actuator actuation sensitivity and bias is only calculated for a actuator actuation input range of 3 V - 10 V, since the 3 V is the minimal amount of voltage needed to get the pump to work</t>
   </si>
 </sst>
 </file>
@@ -395,13 +401,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.86"/>
@@ -482,22 +488,22 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="3" t="s">
@@ -506,7 +512,7 @@
       <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
@@ -538,6 +544,12 @@
       </c>
       <c r="AG1" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -555,15 +567,15 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
+      <c r="W2" s="3"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
@@ -574,16 +586,18 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>140</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>9</v>
@@ -592,7 +606,7 @@
         <v>190</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>0.13</v>
@@ -601,76 +615,82 @@
         <v>1.3</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>37</v>
+      <c r="N3" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="O3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="0" t="n">
         <f aca="false">1400/60</f>
         <v>23.3333333333333</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="R3" s="0" t="n">
         <f aca="false">4450/60</f>
         <v>74.1666666666667</v>
       </c>
-      <c r="Q3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="0" t="n">
-        <f aca="false">(M3-L3)/(P3-O3)</f>
+      <c r="S3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <f aca="false">(M3-O3)/(R3-Q3)</f>
         <v>0.137704918032787</v>
       </c>
-      <c r="S3" s="0" t="n">
-        <f aca="false">M3-(R3*P3)</f>
+      <c r="U3" s="0" t="n">
+        <f aca="false">M3-(T3*R3)</f>
         <v>-0.21311475409836</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V3" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="X3" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" s="0" t="n">
         <v>1000000</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z3" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="AA3" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AB3" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="AE3" s="0" t="s">
+      <c r="AC3" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="AF3" s="0" t="s">
+      <c r="AD3" s="4" t="s">
         <v>46</v>
+      </c>
+      <c r="AG3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>9</v>
@@ -679,7 +699,7 @@
         <v>85</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>0.13</v>
@@ -688,76 +708,82 @@
         <v>0.78</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="N4" s="0" t="s">
-        <v>37</v>
+      <c r="N4" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="O4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="0" t="n">
         <f aca="false">1400/60</f>
         <v>23.3333333333333</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="R4" s="0" t="n">
         <f aca="false">3400/60</f>
         <v>56.6666666666667</v>
       </c>
-      <c r="Q4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="R4" s="0" t="n">
-        <f aca="false">(M4-L4)/(P4-O4)</f>
+      <c r="S4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <f aca="false">(M4-O4)/(R4-Q4)</f>
         <v>0.21</v>
       </c>
-      <c r="S4" s="0" t="n">
-        <f aca="false">M4-(R4*P4)</f>
+      <c r="U4" s="0" t="n">
+        <f aca="false">M4-(T4*R4)</f>
         <v>-1.9</v>
       </c>
-      <c r="T4" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V4" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="X4" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z4" s="0" t="n">
         <v>1000000</v>
-      </c>
-      <c r="Y4" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z4" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="AA4" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="AB4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE4" s="0" t="s">
+      <c r="AB4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC4" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="AF4" s="0" t="s">
-        <v>50</v>
+      <c r="AD4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH4" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>30</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>9</v>
@@ -766,7 +792,7 @@
         <v>38</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>0.13</v>
@@ -775,69 +801,75 @@
         <v>0.35</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M5" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="N5" s="0" t="s">
-        <v>37</v>
+      <c r="N5" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="O5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q5" s="0" t="n">
         <f aca="false">1400/60</f>
         <v>23.3333333333333</v>
       </c>
-      <c r="P5" s="0" t="n">
+      <c r="R5" s="0" t="n">
         <f aca="false">2800/60</f>
         <v>46.6666666666667</v>
       </c>
-      <c r="Q5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="R5" s="0" t="n">
-        <f aca="false">(M5-L5)/(P5-O5)</f>
+      <c r="S5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <f aca="false">(M5-O5)/(R5-Q5)</f>
         <v>0.3</v>
       </c>
-      <c r="S5" s="0" t="n">
-        <f aca="false">M5-(R5*P5)</f>
+      <c r="U5" s="0" t="n">
+        <f aca="false">M5-(T5*R5)</f>
         <v>-4</v>
       </c>
-      <c r="T5" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V5" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="X5" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z5" s="0" t="n">
         <v>1000000</v>
-      </c>
-      <c r="Y5" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z5" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="AA5" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="AB5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE5" s="0" t="s">
+      <c r="AB5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC5" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="AF5" s="0" t="s">
-        <v>54</v>
+      <c r="AD5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG5" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH5" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="35">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -871,11 +903,13 @@
     <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AB3" r:id="rId1" display="..\3_Konzipieren und Konstruieren\Datenblaetter\info_240917_Datenblatt_Pumpe_Wilo_Stratos_25_1-10-2313.pdf"/>
-    <hyperlink ref="AB4" r:id="rId2" display="..\3_Konzipieren und Konstruieren\Datenblaetter\info_240917_Datenblatt_Pumpe_Wilo_Stratos_25_1-6.pdf"/>
-    <hyperlink ref="AB5" r:id="rId3" display="..\3_Konzipieren und Konstruieren\Datenblaetter\info_241024_Datenblatt_Pumpe_Wilo_Stratos_25_1-4.pdf"/>
+    <hyperlink ref="AD3" r:id="rId1" display="..\3_Konzipieren und Konstruieren\Datenblaetter\info_240917_Datenblatt_Pumpe_Wilo_Stratos_25_1-10-2313.pdf"/>
+    <hyperlink ref="AD4" r:id="rId2" display="..\3_Konzipieren und Konstruieren\Datenblaetter\info_240917_Datenblatt_Pumpe_Wilo_Stratos_25_1-6.pdf"/>
+    <hyperlink ref="AD5" r:id="rId3" display="..\3_Konzipieren und Konstruieren\Datenblaetter\info_241024_Datenblatt_Pumpe_Wilo_Stratos_25_1-4.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>